<commit_message>
adding on Pickup Returns Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Eric/Project 2/Pickup Returns Analysis.xlsx
+++ b/Eric/Project 2/Pickup Returns Analysis.xlsx
@@ -8,35 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Music\StudentsWork-Lessons-\Eric\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D122243-F7BA-4AC9-A881-8E13F9206523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CB4FB0-0303-4ACB-BC74-22EF506E9DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Building the House" sheetId="2" r:id="rId2"/>
-    <sheet name="SUM OF SPECIFIC COST ITEM" sheetId="4" r:id="rId3"/>
-    <sheet name="AVERAGE AMOUNT USED IN ROOF" sheetId="6" r:id="rId4"/>
-    <sheet name="AVERAGE AMOUNT USED IN RENTAL" sheetId="8" r:id="rId5"/>
-    <sheet name="TOTAL AMOUNT USED IN RENTAL" sheetId="7" r:id="rId6"/>
-    <sheet name="TOTAL AMOUNT OF ROOF  " sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
+    <sheet name="SUM OF SPECIFIC COST ITEM" sheetId="4" r:id="rId4"/>
+    <sheet name="AVERAGE AMOUNT USED IN ROOF" sheetId="6" r:id="rId5"/>
+    <sheet name="AVERAGE AMOUNT USED IN RENTAL" sheetId="8" r:id="rId6"/>
+    <sheet name="TOTAL AMOUNT USED IN RENTAL" sheetId="7" r:id="rId7"/>
+    <sheet name="TOTAL AMOUNT OF ROOF  " sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Building the House'!$A$1:$E$119</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'TOTAL AMOUNT OF ROOF  '!$A$1:$C$119</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'TOTAL AMOUNT USED IN RENTAL'!$A$1:$A$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'TOTAL AMOUNT OF ROOF  '!$A$1:$C$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'TOTAL AMOUNT USED IN RENTAL'!$A$1:$A$119</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="4" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="5" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="231">
   <si>
     <t>Type</t>
   </si>
@@ -1499,6 +1501,475 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Pickup Returns Analysis.xlsx]Sheet2!PivotTable1</c:name>
+    <c:fmtId val="8"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$4:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Additional Metal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ceiling</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Coop</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Electricals</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Flowers for the coridor rails</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Foundation</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>House Body</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Interiors</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Key</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Plumbing</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Rental</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Roof</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Slab</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Tree</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Windows and Doors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>201540</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45070</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>176720</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AB4-45C5-A1D7-5207D6C0F7F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="878354192"/>
+        <c:axId val="881882544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="878354192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="881882544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="881882544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="878354192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:overlay val="0"/>
@@ -1706,7 +2177,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2091,7 +2562,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2604,6 +3075,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4671,6 +5182,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4755,6 +5769,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF81376-A143-DA7B-3A31-591ECA2F67D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>396875</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -4828,7 +5883,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5007,6 +6062,46 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="BLUEDROP" refreshedDate="45012.927793055555" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="118" xr:uid="{D1531236-397E-4DCF-82DE-B06ED47363BA}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C119" sheet="SUM OF SPECIFIC COST ITEM"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Specific Cost Item" numFmtId="0">
+      <sharedItems count="15">
+        <s v="Tree"/>
+        <s v="Coop"/>
+        <s v="Foundation"/>
+        <s v="House Body"/>
+        <s v="Rental"/>
+        <s v="Interiors"/>
+        <s v="Slab"/>
+        <s v="Electricals"/>
+        <s v="Roof"/>
+        <s v="Plumbing"/>
+        <s v="Ceiling"/>
+        <s v="Windows and Doors"/>
+        <s v="Additional Metal"/>
+        <s v="Flowers for the coridor rails"/>
+        <s v="Key"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Details" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Amount" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="150" maxValue="82000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="118">
   <r>
@@ -6519,6 +7614,601 @@
     <x v="4"/>
     <s v="rented wood for making rentals"/>
     <n v="2000"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="118">
+  <r>
+    <x v="0"/>
+    <s v="Cut trees"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Tree"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="split trunks(kata kuni)"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Remove chicken coop and charcoal burning"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="for the trenches"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="for the trenches"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="for the trenches @ 50 bob a foot"/>
+    <n v="8500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Sand"/>
+    <n v="16000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Sand"/>
+    <n v="16000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Naivasha stones"/>
+    <n v="30000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Ballast"/>
+    <n v="13000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Ballast"/>
+    <n v="13000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Hardcore"/>
+    <n v="9000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Cement"/>
+    <n v="18900"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="for the cementing of the trenches"/>
+    <n v="9000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="for foundation wall day1"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Instead of Whooping wire"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="For carrying the sand-cement mixure to the trenches"/>
+    <n v="900"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Addition "/>
+    <n v="6000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="For the Foundation day 2"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="1 fundi five men@1500 &amp; 600 resp"/>
+    <n v="4500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="addition 100ft"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="For foundation soil"/>
+    <n v="4500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="For foundation soil"/>
+    <n v="4500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="For foundation soil"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Hardcore for the house"/>
+    <n v="4500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Additional HArdcore &amp; leveling"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="D10"/>
+    <n v="12600"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="D8"/>
+    <n v="8170"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Binding Wire"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Cement"/>
+    <n v="18900"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Stones( Machine Cut)"/>
+    <n v="67500"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Electric pipes"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Miscelaneous"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="addition for the remaining part of the house"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Both 3 and 4 inches"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="laying electrical pipes in the slab"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Laying the Slab"/>
+    <n v="7100"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="paper for partitioning teh house"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Laying the first 2 courses"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Two brooms for sweeping the  sand"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Laying 3 courses of stones"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Laying 2 courses of stones"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Laying 2 courses of stones"/>
+    <n v="6300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Supervision"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="For the Rentals"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="For the rentals"/>
+    <n v="1250"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Finalize house and Rentals"/>
+    <n v="5100"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="undocumented spendings"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="dividing the house"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="For the rentals"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Rentals Day 1"/>
+    <n v="4800"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Day 2"/>
+    <n v="4800"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Day 3"/>
+    <n v="4200"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="rented wood for making rentals"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="For rental wood 300,for metal rods 300, other 300"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Cleaning the area,sweeping the sand, arrranging the remaining stones etc"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Other unmentioned costs"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="3X2 (1300ft),2X2 (500ft),fesia(200ft)"/>
+    <n v="82000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Fundi( for assistance)"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Transport and Lunch"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="4kg(4&quot;),4kgs(3&quot;),2kg(2&quot;)"/>
+    <n v="1600"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="For drilling the holes for the sockets"/>
+    <n v="1800"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Addition Nails"/>
+    <n v="1600"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="for a termite resistant house"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="for the walls +transport"/>
+    <n v="6000"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="pipes and transport"/>
+    <n v="12700"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="2x2 wood for ceiling"/>
+    <n v="24100"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Roof Mbao and Door Frames and Nails"/>
+    <n v="5830"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="all metals for the windows"/>
+    <n v="42000"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="deposit"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="for electric pipes installation"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Deposit"/>
+    <n v="25000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="to buy mambati in ruiru"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Mambati - Boxprofile"/>
+    <n v="53990"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Added 1 to finalize"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="for the main door"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="for the undercoat/windows and doors"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="Addition Tubes "/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="For the sideboards in the roof, 100 ft for the tank"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <s v="for the doors"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <s v="11 pieces @600"/>
+    <n v="6600"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="to put up the windows and doors (2 days)"/>
+    <n v="3600"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="for the plastering @ 1 lorry (8000 owed previously)"/>
+    <n v="8000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="for the plastering @ 30 pcs"/>
+    <n v="18900"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="ventilations @50,hole pass for frames etc"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="1 fundi 1 labouror plastering 2 days (mon -teu)"/>
+    <n v="3600"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="plastering wed-sat"/>
+    <n v="7200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="plastering  (1 week)"/>
+    <n v="10800"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="plastering finalize (contract)"/>
+    <n v="12000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="tiles for living rool,kitchen ,corridor and bathroom"/>
+    <n v="30690"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="for the floor and tiles"/>
+    <n v="25050"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="metal rods,brushes ,gauze etc for finishings"/>
+    <n v="2500"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="for the dining window(sold at a discount)"/>
+    <n v="6000"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <s v="drilling trenches for Key decorations"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <s v="drilling trenches for Key decorations"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <s v="Working on the Keys"/>
+    <n v="14400"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Floor - leveling for the entire house"/>
+    <n v="4200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Creating Kitchen tabletop"/>
+    <n v="3600"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="for the window panes at 125 per sq. ft and free labour (11200) + Bat for stickung 3500 + 3 silicon ( at 350 each)"/>
+    <n v="15000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="labour for the tiles 2 fundis and 2 laborors @ 1200,600 resp"/>
+    <n v="15000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="for the tiles"/>
+    <n v="3200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="binders $ bathroom drainage with pipes"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Sink for the kitchen table top"/>
+    <n v="2100"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="finalizing kitchen tiling"/>
+    <n v="2200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Undercoat Paint"/>
+    <n v="7700"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Filler for the paint"/>
+    <n v="7500"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="toilet drainage for the bathroom"/>
+    <n v="800"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="undercoat - full  house "/>
+    <n v="1300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Scheming (full house)"/>
+    <n v="3900"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Outside the house and fesia board &amp; sitting and Kitchen silk paint"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="3 cans of 4litre silk paints @ 1850 each"/>
+    <n v="5700"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Miscelaneous costs for black paper,sand papers,rollers,brush etc"/>
+    <n v="2500"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Paint the  silk paint"/>
+    <n v="3900"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="wiring the house at a cost of 100 per metre, 40 meters for 10 mm wire"/>
+    <n v="7000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="small stuff like  cutoffs,bulbs ,holders ,wiring labor ,etc"/>
+    <n v="9000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Lock for the house "/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="pay labor for final sandpaper job"/>
+    <n v="500"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -6750,6 +8440,115 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAE85A4B-5A07-42C8-849B-CECF1AC9CE26}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="12"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="8" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0F272C5E-E5CE-432A-B283-6293447AD54B}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -6813,8 +8612,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E1C38D2-0756-452D-80AB-EBCC91C38354}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E1C38D2-0756-452D-80AB-EBCC91C38354}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -9094,7 +10893,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="65.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:5" ht="63" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>190</v>
       </c>
@@ -13829,6 +15628,162 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8379AD9C-6CF2-493B-A6B8-B0178820E1E3}">
+  <dimension ref="A3:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="111" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="13">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="13">
+        <v>24100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="13">
+        <v>26300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="13">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="13">
+        <v>150100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="13">
+        <v>153100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="13">
+        <v>201540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="13">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="13">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="13">
+        <v>45070</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="13">
+        <v>176720</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="13">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="13">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="13">
+        <v>67800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="13">
+        <v>904030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C964FF48-44CA-41E8-92AC-869A1015D329}">
   <dimension ref="A1:C120"/>
   <sheetViews>
@@ -15176,7 +17131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C48AADB-E13A-4B3B-A1A3-669E7DAE0DE4}">
   <dimension ref="A3:B5"/>
   <sheetViews>
@@ -15206,7 +17161,7 @@
       <c r="A4" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4">
         <v>16065.454545454546</v>
       </c>
     </row>
@@ -15214,7 +17169,7 @@
       <c r="A5" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>16065.454545454546</v>
       </c>
     </row>
@@ -15224,7 +17179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F8B385-283C-4385-9F10-3FD4305CE7CE}">
   <dimension ref="A3:B5"/>
   <sheetViews>
@@ -15257,7 +17212,7 @@
       <c r="A4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4">
         <v>4097.272727272727</v>
       </c>
     </row>
@@ -15265,7 +17220,7 @@
       <c r="A5" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>4097.272727272727</v>
       </c>
     </row>
@@ -15275,12 +17230,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD272A8-201B-4534-A517-C7DCC672C932}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="180" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="180" workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -16617,7 +18572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6549D1BB-3141-4FD3-B297-6C0B1D1F9287}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C121"/>

</xml_diff>